<commit_message>
Updated tables for patient care
</commit_message>
<xml_diff>
--- a/technical/design/database/database_schema.xlsx
+++ b/technical/design/database/database_schema.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
   <si>
     <t>Database</t>
   </si>
@@ -302,13 +302,157 @@
   </si>
   <si>
     <t>devstate</t>
+  </si>
+  <si>
+    <t>spl_hpft_master</t>
+  </si>
+  <si>
+    <t>spl_hpft_master_task_lib_tbl</t>
+  </si>
+  <si>
+    <t>spl_prod_master_config</t>
+  </si>
+  <si>
+    <t>spl_prod_master_serv_conf_type_tbl</t>
+  </si>
+  <si>
+    <t>spl_prod_master_sp_category_tbl</t>
+  </si>
+  <si>
+    <t>spl_hpft_node_xxxx</t>
+  </si>
+  <si>
+    <t>spl_node_task_lib_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_service_instance_tbl</t>
+  </si>
+  <si>
+    <t>spl_hpft_patient_master_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_cpm_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_dev_sp_mapping</t>
+  </si>
+  <si>
+    <t>spl_node_dev_status_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_dev_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_feedback_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_field_operator_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_fop_sp_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_report_template_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_service_conf_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_service_in_txn_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_sp_category_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_sp_complaint_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_sp_tbl</t>
+  </si>
+  <si>
+    <t>spl_node_sync_config_tbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> devsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> devstate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fop</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fopsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> report</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> serv_conf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> serv_in_txn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> serv_conf_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spcomplaint</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sync</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> task</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> patient</t>
+  </si>
+  <si>
+    <t>spl_node_user_tbl</t>
+  </si>
+  <si>
+    <t>this tbl hold user_id from spl database and other fields required locally</t>
+  </si>
+  <si>
+    <t>spl_node_patient_usr_mapping</t>
+  </si>
+  <si>
+    <t>patusr</t>
+  </si>
+  <si>
+    <t>spl_node_patient_sp_mapping</t>
+  </si>
+  <si>
+    <t>patsp</t>
+  </si>
+  <si>
+    <t>spl_node_user_status_tbl</t>
+  </si>
+  <si>
+    <t>usrstate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -438,6 +582,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,11 +597,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,6 +606,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -505,7 +660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,9 +692,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,6 +727,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -746,21 +903,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="62.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.1796875" customWidth="1"/>
+    <col min="6" max="6" width="62.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -777,16 +936,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="2"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
@@ -799,7 +958,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
@@ -812,7 +971,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -827,11 +986,11 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>91</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -840,11 +999,11 @@
       <c r="E7" s="2"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -853,7 +1012,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
@@ -866,7 +1025,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -881,7 +1040,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
@@ -896,11 +1055,11 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -909,7 +1068,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -922,7 +1081,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -937,11 +1096,11 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -950,11 +1109,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -963,7 +1122,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
@@ -978,7 +1137,7 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
@@ -991,7 +1150,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1004,7 +1163,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1017,7 +1176,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1030,7 +1189,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="2:6" ht="45">
+    <row r="22" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1041,16 +1200,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="2"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1065,7 +1224,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1080,7 +1239,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1095,16 +1254,16 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="2"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1114,10 +1273,10 @@
       <c r="D28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="13"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1132,7 +1291,7 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1147,7 +1306,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
@@ -1162,11 +1321,11 @@
       </c>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1177,7 +1336,7 @@
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1351,7 @@
       </c>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="2:6" ht="45">
+    <row r="34" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>28</v>
       </c>
@@ -1209,7 +1368,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="30">
+    <row r="35" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -1219,18 +1378,18 @@
       <c r="D35" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1241,16 +1400,16 @@
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="8" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="2"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
         <v>84</v>
@@ -1261,7 +1420,7 @@
       </c>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>84</v>
@@ -1272,7 +1431,7 @@
       </c>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
         <v>84</v>
@@ -1283,7 +1442,7 @@
       </c>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
         <v>84</v>
@@ -1294,12 +1453,351 @@
       </c>
       <c r="F41" s="6"/>
     </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B65" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B66" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B67" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B68" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B47:D47"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1307,24 +1805,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>